<commit_message>
username and password field resets after login
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 1 Project Documentation.xlsx
+++ b/CSSECDV - Case Study 1 Project Documentation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CSSECDV\CSSECDV-Case-Study-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3A98B0-0A51-4B17-B79F-83F0A0D11B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB63C2B-AC35-4F60-8E50-33369207787E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Security Issue</t>
   </si>
@@ -69,14 +69,38 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Unmasked password login field.</t>
-  </si>
-  <si>
     <t>Login.java</t>
   </si>
   <si>
     <t>Password needs to be masked to prevent the vulnerabilities mentioned
 Change the password field from javax.swing.JTextField(); to javax.swing.JPasswordField();</t>
+  </si>
+  <si>
+    <t>Sets the fields to an empty string after clicking login button: frame.loginPnl.usernameFld.setText("");
+frame.loginPnl.passwordFld.setText("");</t>
+  </si>
+  <si>
+    <t>Allows unauthorized user/s to relogin with the previous credentials of a recent user</t>
+  </si>
+  <si>
+    <t>Not clearing login fields</t>
+  </si>
+  <si>
+    <t>Allows unauthorized user/s to login without having the need to input valid user credentials</t>
+  </si>
+  <si>
+    <t>Unmasked password login field</t>
+  </si>
+  <si>
+    <t>No login verification</t>
+  </si>
+  <si>
+    <t>Login.java, Main.java</t>
+  </si>
+  <si>
+    <t>Added event listener to login button that checks if the inputted username and password matches an existing account stored in the database. 
+Method implemented:
+public boolean validateLogin(String username, String password)</t>
   </si>
 </sst>
 </file>
@@ -267,18 +291,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -291,16 +303,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -623,7 +647,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -631,231 +655,247 @@
     <col min="1" max="1" width="7.69921875" customWidth="1"/>
     <col min="2" max="2" width="40.796875" customWidth="1"/>
     <col min="3" max="3" width="20.796875" customWidth="1"/>
-    <col min="4" max="4" width="40.796875" customWidth="1"/>
+    <col min="4" max="4" width="65.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="13" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>19</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added input validation in registration
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 1 Project Documentation.xlsx
+++ b/CSSECDV - Case Study 1 Project Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CSSECDV\CSSECDV-Case-Study-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB63C2B-AC35-4F60-8E50-33369207787E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD40FC6-F238-4658-A11B-D628490631C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Security Issue</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Register.java</t>
-  </si>
-  <si>
-    <t>Unmasked password registration fields.</t>
   </si>
   <si>
     <t xml:space="preserve">Shoulder surfing when a user is typing his/her password:
@@ -66,18 +63,11 @@
 Change from password = new javax.swing.JTextField(); to password = new javax.swing.JPasswordField();</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Login.java</t>
   </si>
   <si>
     <t>Password needs to be masked to prevent the vulnerabilities mentioned
 Change the password field from javax.swing.JTextField(); to javax.swing.JPasswordField();</t>
-  </si>
-  <si>
-    <t>Sets the fields to an empty string after clicking login button: frame.loginPnl.usernameFld.setText("");
-frame.loginPnl.passwordFld.setText("");</t>
   </si>
   <si>
     <t>Allows unauthorized user/s to relogin with the previous credentials of a recent user</t>
@@ -101,31 +91,45 @@
     <t>Added event listener to login button that checks if the inputted username and password matches an existing account stored in the database. 
 Method implemented:
 public boolean validateLogin(String username, String password)</t>
+  </si>
+  <si>
+    <t>Not clearing registration fields</t>
+  </si>
+  <si>
+    <t>Unmasked password registration fields</t>
+  </si>
+  <si>
+    <t>Usernames are case-sensitive</t>
+  </si>
+  <si>
+    <t>Multiple users with the same username but in different cases can exist</t>
+  </si>
+  <si>
+    <t>Use toLowerCase() on the user name value before storing in the database</t>
+  </si>
+  <si>
+    <t>Exposes username of the recently registered user</t>
+  </si>
+  <si>
+    <t>Sets the fields to an empty string after clicking login button: 
+frame.loginPnl.usernameFld.setText("");
+frame.loginPnl.passwordFld.setText("");</t>
+  </si>
+  <si>
+    <t>Sets the fields to an empty string after clicking register button: 
+frame.registerPnl.usernameFld.setText("");
+frame.registerPnl.passwordFld.setText("");
+frame.registerPnl.confpassFld.setText("");</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,36 +293,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -641,13 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ADE879-4575-BE42-ACF5-88079327BE13}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -660,242 +655,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>9</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>10</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>11</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
-        <v>13</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
-        <v>14</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
-        <v>15</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
-        <v>16</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
-        <v>17</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
-        <v>18</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>19</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>